<commit_message>
Fold  / Mirror tested, implemented
</commit_message>
<xml_diff>
--- a/20_LogicPaper_cyborg.xlsx
+++ b/20_LogicPaper_cyborg.xlsx
@@ -617,10 +617,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>F4-F</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>y</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -856,13 +852,18 @@
     <t>, where U is an unitary matrix;</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>F4 vs F</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.E+00"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1224,7 +1225,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1381,6 +1382,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1444,7 +1451,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1525,16 +1531,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.5102082659902809</c:v>
+                  <c:v>2.0889778458011876</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2718260829946573</c:v>
+                  <c:v>1.9705871649346041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.8108346089642815</c:v>
+                  <c:v>8.0226259239104625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19804799880622892</c:v>
+                  <c:v>4.8865644968208333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1546,16 +1552,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.1049263847858963</c:v>
+                  <c:v>5.7877612467890316</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5723103907888909</c:v>
+                  <c:v>9.6263577248062244</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.2843475518953351</c:v>
+                  <c:v>4.0406923545963487</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33973694636738605</c:v>
+                  <c:v>2.1618380439278209</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1607,16 +1613,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-3.5621289850828188</c:v>
+                  <c:v>-0.14866299990686294</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7533066719188311</c:v>
+                  <c:v>3.5695390096322859</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.593995930952314E-2</c:v>
+                  <c:v>-3.4872705982824352</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4.8493059711530533</c:v>
+                  <c:v>-4.4128735369391254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1628,16 +1634,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.15917932309072</c:v>
+                  <c:v>7.4659918810700692</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.461199949095761</c:v>
+                  <c:v>8.4271438412829625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.578018539136403</c:v>
+                  <c:v>12.673114746241021</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.125252423836848</c:v>
+                  <c:v>9.136416569247789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1722,11 +1728,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="417917840"/>
-        <c:axId val="417923280"/>
+        <c:axId val="-1549920256"/>
+        <c:axId val="-1549918624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417917840"/>
+        <c:axId val="-1549920256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,12 +1789,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417923280"/>
+        <c:crossAx val="-1549918624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="417923280"/>
+        <c:axId val="-1549918624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1845,7 +1851,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417917840"/>
+        <c:crossAx val="-1549920256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1859,7 +1865,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1943,7 +1948,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>fold!$B$173</c:f>
+          <c:f>fold!$B$181</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -1952,6 +1957,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1990,6 +1996,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>CP</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2004,36 +2013,36 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>fold!$C$175:$E$175</c:f>
+              <c:f>fold!$C$183:$E$183</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.138764837597531</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36387285617567211</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.79728643537602606</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fold!$C$176:$E$176</c:f>
+              <c:f>fold!$C$184:$E$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.35725188541231967</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1319341123135287</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5823618789290359</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2043,6 +2052,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>MODEL</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2057,36 +2069,36 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>fold!$C$179:$E$179</c:f>
+              <c:f>fold!$C$187:$E$187</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.82681583615392751</c:v>
+                  <c:v>-1.1999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88316473916052796</c:v>
+                  <c:v>1.1102230246251565E-16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18643686423655009</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fold!$C$180:$E$180</c:f>
+              <c:f>fold!$C$188:$E$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0915249924373929</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7780500811090254</c:v>
+                  <c:v>0.40000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8103999934929003</c:v>
+                  <c:v>-0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2094,6 +2106,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2101,15 +2114,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="417924368"/>
-        <c:axId val="417928176"/>
+        <c:axId val="-1549916992"/>
+        <c:axId val="-1549915904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417924368"/>
+        <c:axId val="-1549916992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="-1"/>
+          <c:max val="3"/>
+          <c:min val="-3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2164,16 +2177,16 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417928176"/>
+        <c:crossAx val="-1549915904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="417928176"/>
+        <c:axId val="-1549915904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="-1"/>
+          <c:max val="3"/>
+          <c:min val="-3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2228,7 +2241,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417924368"/>
+        <c:crossAx val="-1549916992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2240,6 +2253,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2515,11 +2560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="630034656"/>
-        <c:axId val="630024320"/>
+        <c:axId val="-1550576848"/>
+        <c:axId val="-1315009536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="630034656"/>
+        <c:axId val="-1550576848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2576,12 +2621,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="630024320"/>
+        <c:crossAx val="-1315009536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="630024320"/>
+        <c:axId val="-1315009536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +2683,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="630034656"/>
+        <c:crossAx val="-1550576848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16067,8 +16112,8 @@
       <xdr:rowOff>21981</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2121158" cy="1307794"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="テキスト ボックス 24"/>
@@ -16995,7 +17040,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="テキスト ボックス 24"/>
@@ -20291,8 +20336,8 @@
       <xdr:rowOff>139211</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2694840" cy="546560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -20729,7 +20774,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -22063,8 +22108,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2417885" y="19423671"/>
-          <a:ext cx="1714499" cy="586156"/>
+          <a:off x="2623038" y="19423671"/>
+          <a:ext cx="1714500" cy="586156"/>
           <a:chOff x="1069731" y="18441865"/>
           <a:chExt cx="1296865" cy="586154"/>
         </a:xfrm>
@@ -22158,7 +22203,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="5771715">
-          <a:off x="5369169" y="19436861"/>
+          <a:off x="5574323" y="19436861"/>
           <a:ext cx="1296865" cy="586154"/>
           <a:chOff x="1069731" y="18441865"/>
           <a:chExt cx="1296865" cy="586154"/>
@@ -28989,8 +29034,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5216043" cy="975716"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="37" name="テキスト ボックス 36"/>
@@ -29737,7 +29782,7 @@
                                   </m:e>
                                   <m:e>
                                     <m:r>
-                                      <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1800" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                                      <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                                         <a:ln>
                                           <a:noFill/>
                                         </a:ln>
@@ -31185,7 +31230,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="37" name="テキスト ボックス 36"/>
@@ -31250,7 +31295,7 @@
                 <a:t>𝑈 ̂=1/(〈〖𝑑^′〗_2 ┤| 𝜎 ̂_𝑦 ├|〖𝑑^′〗_1 〉 ) 𝜎 ̂_𝑦 (├|〖𝑑^′〗_1 〉 (█(0@</a:t>
               </a:r>
               <a:r>
-                <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
@@ -31367,15 +31412,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>249117</xdr:colOff>
-      <xdr:row>172</xdr:row>
-      <xdr:rowOff>175847</xdr:rowOff>
+      <xdr:colOff>293078</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>542194</xdr:colOff>
-      <xdr:row>185</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>805962</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>219808</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -31392,6 +31437,116 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>603432</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>153863</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>149468</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>33702</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="図 38"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1980894" y="32897882"/>
+          <a:ext cx="3004343" cy="3023089"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>29137</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>614729</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>21248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="図 40"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5553637" y="33813750"/>
+          <a:ext cx="2651784" cy="1852979"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -37403,68 +37558,68 @@
   <sheetData>
     <row r="1" spans="1:3" s="50" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" s="51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -37486,7 +37641,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="50" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
@@ -37497,22 +37652,22 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -37534,44 +37689,44 @@
   <sheetData>
     <row r="1" spans="1:3" s="50" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -37586,8 +37741,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H174"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B105" sqref="A103:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -37677,7 +37832,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.4">
@@ -37854,19 +38009,19 @@
       </c>
       <c r="E106" s="2">
         <f t="shared" ref="E106:F109" ca="1" si="0">RAND()*10</f>
-        <v>8.5102082659902809</v>
+        <v>2.0889778458011876</v>
       </c>
       <c r="F106" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1049263847858963</v>
+        <v>5.7877612467890316</v>
       </c>
       <c r="G106" s="2">
         <f t="array" aca="1" ref="G106:H106" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E106:F106)))+V_NN</f>
-        <v>-3.5621289850828188</v>
+        <v>-0.14866299990686294</v>
       </c>
       <c r="H106" s="2">
         <f ca="1"/>
-        <v>13.15917932309072</v>
+        <v>7.4659918810700692</v>
       </c>
     </row>
     <row r="107" spans="3:8" x14ac:dyDescent="0.4">
@@ -37876,19 +38031,19 @@
       </c>
       <c r="E107" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2718260829946573</v>
+        <v>1.9705871649346041</v>
       </c>
       <c r="F107" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5723103907888909</v>
+        <v>9.6263577248062244</v>
       </c>
       <c r="G107" s="2">
         <f t="array" aca="1" ref="G107:H107" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E107:F107)))+V_NN</f>
-        <v>1.7533066719188311</v>
+        <v>3.5695390096322859</v>
       </c>
       <c r="H107" s="2">
         <f ca="1"/>
-        <v>14.461199949095761</v>
+        <v>8.4271438412829625</v>
       </c>
     </row>
     <row r="108" spans="3:8" x14ac:dyDescent="0.4">
@@ -37898,19 +38053,19 @@
       </c>
       <c r="E108" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8108346089642815</v>
+        <v>8.0226259239104625</v>
       </c>
       <c r="F108" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2843475518953351</v>
+        <v>4.0406923545963487</v>
       </c>
       <c r="G108" s="2">
         <f t="array" aca="1" ref="G108:H108" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E108:F108)))+V_NN</f>
-        <v>8.593995930952314E-2</v>
+        <v>-3.4872705982824352</v>
       </c>
       <c r="H108" s="2">
         <f ca="1"/>
-        <v>15.578018539136403</v>
+        <v>12.673114746241021</v>
       </c>
     </row>
     <row r="109" spans="3:8" x14ac:dyDescent="0.4">
@@ -37920,19 +38075,19 @@
       </c>
       <c r="E109" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19804799880622892</v>
+        <v>4.8865644968208333</v>
       </c>
       <c r="F109" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33973694636738605</v>
+        <v>2.1618380439278209</v>
       </c>
       <c r="G109" s="2">
         <f t="array" aca="1" ref="G109:H109" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E109:F109)))+V_NN</f>
-        <v>-4.8493059711530533</v>
+        <v>-4.4128735369391254</v>
       </c>
       <c r="H109" s="2">
         <f ca="1"/>
-        <v>4.125252423836848</v>
+        <v>9.136416569247789</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.4">
@@ -38021,15 +38176,15 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L197"/>
+  <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J54" sqref="E50:J54"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D192" activeCellId="1" sqref="E196:E197 D192:D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
     <col min="4" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -38087,7 +38242,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="C40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
@@ -38247,12 +38402,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C133" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>89</v>
       </c>
@@ -38261,248 +38416,64 @@
       <c r="E137" s="24"/>
       <c r="F137" s="24"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C138" s="24"/>
       <c r="D138" s="24"/>
       <c r="E138" s="24"/>
       <c r="F138" s="24"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B139" t="s">
-        <v>126</v>
-      </c>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C139" s="24"/>
       <c r="D139" s="24"/>
       <c r="E139" s="24"/>
       <c r="F139" s="24"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B140" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K140" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="L140" s="22"/>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C140" s="24"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="24"/>
+      <c r="F140" s="24"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B141" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C141" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>8.099657249437997E-2</v>
-      </c>
-      <c r="D141" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.28811422392566799</v>
-      </c>
-      <c r="E141" s="2">
-        <f ca="1">D141-C141</f>
-        <v>0.20711765143128802</v>
-      </c>
-      <c r="F141" s="2">
-        <f ca="1">-E142</f>
-        <v>-0.35699938509916063</v>
-      </c>
-      <c r="G141" s="2">
-        <f t="array" aca="1" ref="G141:H142" ca="1">{1,0;0,1}-2*(F141:F142*TRANSPOSE(F141:F142))/(F141^2+F142^2)</f>
-        <v>-0.49634684237358995</v>
-      </c>
-      <c r="H141" s="2">
-        <f ca="1"/>
-        <v>0.86812430680506059</v>
-      </c>
-      <c r="I141" s="2">
-        <f t="array" aca="1" ref="I141:I142" ca="1">2*F141:F142*SUMPRODUCT(F141:F142,C141:C142)/(F141^2+F142^2)</f>
-        <v>0.26170857228315453</v>
-      </c>
-      <c r="K141" s="17">
-        <f t="array" aca="1" ref="K141:L142" ca="1">MMULT(G141:H142,G141:H142)</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="L141" s="17">
-        <f ca="1"/>
-        <v>-1.1102230246251565E-16</v>
-      </c>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C141" s="24"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="24"/>
+      <c r="F141" s="24"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B142" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C142" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>-0.16185424793048364</v>
-      </c>
-      <c r="D142" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.19514513716867699</v>
-      </c>
-      <c r="E142" s="2">
-        <f ca="1">D142-C142</f>
-        <v>0.35699938509916063</v>
-      </c>
-      <c r="F142" s="2">
-        <f ca="1">E141</f>
-        <v>0.20711765143128802</v>
-      </c>
-      <c r="G142" s="2">
-        <f ca="1"/>
-        <v>0.86812430680506059</v>
-      </c>
-      <c r="H142" s="2">
-        <f ca="1"/>
-        <v>0.49634684237358984</v>
-      </c>
-      <c r="I142" s="2">
-        <f ca="1"/>
-        <v>-0.1518334963957054</v>
-      </c>
-      <c r="K142" s="2">
-        <f ca="1"/>
-        <v>-1.1102230246251565E-16</v>
-      </c>
-      <c r="L142" s="2">
-        <f ca="1"/>
-        <v>1.0000000000000002</v>
-      </c>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C142" s="24"/>
+      <c r="D142" s="24"/>
+      <c r="E142" s="24"/>
+      <c r="F142" s="24"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C143" s="24"/>
       <c r="D143" s="24"/>
       <c r="E143" s="24"/>
       <c r="F143" s="24"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B144" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H144" s="2"/>
-      <c r="I144" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K144" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="L144" s="22"/>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C144" s="24"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="24"/>
+      <c r="F144" s="24"/>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B145" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C145" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.22341027837690475</v>
-      </c>
-      <c r="D145" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>-0.40866214969655679</v>
-      </c>
-      <c r="E145" s="2">
-        <f ca="1">D145-C145</f>
-        <v>-0.63207242807346153</v>
-      </c>
-      <c r="F145" s="2">
-        <f ca="1">-E146</f>
-        <v>-0.11484713640519129</v>
-      </c>
-      <c r="G145" s="2">
-        <f t="array" aca="1" ref="G145:H146" ca="1">{1,0;0,1}-2*(F145:F146*TRANSPOSE(F145:F146))/(F145^2+F146^2)</f>
-        <v>0.9360809714097863</v>
-      </c>
-      <c r="H145" s="2">
-        <f ca="1"/>
-        <v>-0.35178461445110265</v>
-      </c>
-      <c r="I145" s="2">
-        <f t="array" aca="1" ref="I145:I146" ca="1">2*F145:F146*SUMPRODUCT(F145:F146,C145:C146)/(F145^2+F146^2)</f>
-        <v>0.26554314100530263</v>
-      </c>
-      <c r="K145" s="17">
-        <f t="array" aca="1" ref="K145:L146" ca="1">MMULT(G145:H146,G145:H146)</f>
-        <v>1</v>
-      </c>
-      <c r="L145" s="17">
-        <f ca="1"/>
-        <v>-5.5511151231257827E-17</v>
-      </c>
+      <c r="C145" s="24"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="24"/>
+      <c r="F145" s="24"/>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B146" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C146" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.71425230869301326</v>
-      </c>
-      <c r="D146" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.82909944509820455</v>
-      </c>
-      <c r="E146" s="2">
-        <f ca="1">D146-C146</f>
-        <v>0.11484713640519129</v>
-      </c>
-      <c r="F146" s="2">
-        <f ca="1">E145</f>
-        <v>-0.63207242807346153</v>
-      </c>
-      <c r="G146" s="2">
-        <f ca="1"/>
-        <v>-0.35178461445110265</v>
-      </c>
-      <c r="H146" s="2">
-        <f ca="1"/>
-        <v>-0.93608097140978619</v>
-      </c>
-      <c r="I146" s="2">
-        <f ca="1"/>
-        <v>1.4614426022892846</v>
-      </c>
-      <c r="K146" s="2">
-        <f ca="1"/>
-        <v>-5.5511151231257827E-17</v>
-      </c>
-      <c r="L146" s="2">
-        <f ca="1"/>
-        <v>0.99999999999999989</v>
-      </c>
+      <c r="C146" s="24"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="24"/>
+      <c r="F146" s="24"/>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B147" t="s">
+        <v>126</v>
+      </c>
       <c r="C147" s="24"/>
       <c r="D147" s="24"/>
       <c r="E147" s="24"/>
@@ -38510,7 +38481,7 @@
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B148" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>109</v>
@@ -38541,40 +38512,36 @@
         <v>107</v>
       </c>
       <c r="C149" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.70995262908494627</v>
+        <v>-1</v>
       </c>
       <c r="D149" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>-0.48416329072232567</v>
+        <v>1</v>
       </c>
       <c r="E149" s="2">
-        <f ca="1">D149-C149</f>
-        <v>-1.1941159198072719</v>
+        <f>D149-C149</f>
+        <v>2</v>
       </c>
       <c r="F149" s="2">
-        <f ca="1">-E150</f>
-        <v>0.51538754451434698</v>
+        <f>-E150</f>
+        <v>-2</v>
       </c>
       <c r="G149" s="2">
-        <f t="array" aca="1" ref="G149:H150" ca="1">{1,0;0,1}-2*(F149:F150*TRANSPOSE(F149:F150))/(F149^2+F150^2)</f>
-        <v>0.68593734889357971</v>
+        <f t="array" ref="G149:H150">{1,0;0,1}-2*(F149:F150*TRANSPOSE(F149:F150))/(F149^2+F150^2)</f>
+        <v>0</v>
       </c>
       <c r="H149" s="2">
-        <f ca="1"/>
-        <v>0.72766060316114922</v>
+        <v>1</v>
       </c>
       <c r="I149" s="2">
-        <f t="array" aca="1" ref="I149:I150" ca="1">2*F149:F150*SUMPRODUCT(F149:F150,C149:C150)/(F149^2+F150^2)</f>
-        <v>-0.23091608702860345</v>
+        <f t="array" ref="I149:I150">2*F149:F150*SUMPRODUCT(F149:F150,C149:C150)/(F149^2+F150^2)</f>
+        <v>0</v>
       </c>
       <c r="K149" s="17">
-        <f t="array" aca="1" ref="K149:L150" ca="1">MMULT(G149:H150,G149:H150)</f>
+        <f t="array" ref="K149:L150">MMULT(G149:H150,G149:H150)</f>
         <v>1</v>
       </c>
       <c r="L149" s="17">
-        <f ca="1"/>
-        <v>1.1102230246251565E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.4">
@@ -38582,45 +38549,44 @@
         <v>108</v>
       </c>
       <c r="C150" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.62376015673680252</v>
+        <v>-1</v>
       </c>
       <c r="D150" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.10837261222245553</v>
+        <v>1</v>
       </c>
       <c r="E150" s="2">
-        <f ca="1">D150-C150</f>
-        <v>-0.51538754451434698</v>
+        <f>D150-C150</f>
+        <v>2</v>
       </c>
       <c r="F150" s="2">
-        <f ca="1">E149</f>
-        <v>-1.1941159198072719</v>
+        <f>E149</f>
+        <v>2</v>
       </c>
       <c r="G150" s="2">
-        <f ca="1"/>
-        <v>0.72766060316114922</v>
+        <v>1</v>
       </c>
       <c r="H150" s="2">
-        <f ca="1"/>
-        <v>-0.6859373488935796</v>
+        <v>0</v>
       </c>
       <c r="I150" s="2">
-        <f ca="1"/>
-        <v>0.53501598669849304</v>
+        <v>0</v>
       </c>
       <c r="K150" s="2">
-        <f ca="1"/>
-        <v>1.1102230246251565E-16</v>
+        <v>0</v>
       </c>
       <c r="L150" s="2">
-        <f ca="1"/>
-        <v>0.99999999999999978</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C151" s="24"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="24"/>
+      <c r="F151" s="24"/>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B152" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>109</v>
@@ -38651,40 +38617,36 @@
         <v>107</v>
       </c>
       <c r="C153" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>6.5062147488072375E-2</v>
+        <v>-1</v>
       </c>
       <c r="D153" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>-0.3476647889409028</v>
+        <v>1</v>
       </c>
       <c r="E153" s="2">
-        <f ca="1">D153-C153</f>
-        <v>-0.41272693642897518</v>
+        <f>D153-C153</f>
+        <v>2</v>
       </c>
       <c r="F153" s="2">
-        <f ca="1">-E154</f>
-        <v>1.6716827230632201</v>
+        <f>-E154</f>
+        <v>-1</v>
       </c>
       <c r="G153" s="2">
-        <f t="array" aca="1" ref="G153:H154" ca="1">{1,0;0,1}-2*(F153:F154*TRANSPOSE(F153:F154))/(F153^2+F154^2)</f>
-        <v>-0.88509194906478816</v>
+        <f t="array" ref="G153:H154">{1,0;0,1}-2*(F153:F154*TRANSPOSE(F153:F154))/(F153^2+F154^2)</f>
+        <v>0.6</v>
       </c>
       <c r="H153" s="2">
-        <f ca="1"/>
-        <v>0.4654162026624068</v>
+        <v>0.8</v>
       </c>
       <c r="I153" s="2">
-        <f t="array" aca="1" ref="I153:I154" ca="1">2*F153:F154*SUMPRODUCT(F153:F154,C153:C154)/(F153^2+F154^2)</f>
-        <v>-0.29246326361369479</v>
+        <f t="array" ref="I153:I154">2*F153:F154*SUMPRODUCT(F153:F154,C153:C154)/(F153^2+F154^2)</f>
+        <v>0.4</v>
       </c>
       <c r="K153" s="17">
-        <f t="array" aca="1" ref="K153:L154" ca="1">MMULT(G153:H154,G153:H154)</f>
+        <f t="array" ref="K153:L154">MMULT(G153:H154,G153:H154)</f>
         <v>1</v>
       </c>
       <c r="L153" s="17">
-        <f ca="1"/>
-        <v>0</v>
+        <v>-1.1102230246251565E-16</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.4">
@@ -38692,55 +38654,66 @@
         <v>108</v>
       </c>
       <c r="C154" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.89191435892795945</v>
+        <v>-1</v>
       </c>
       <c r="D154" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>-0.77976836413526063</v>
+        <v>0</v>
       </c>
       <c r="E154" s="2">
-        <f ca="1">D154-C154</f>
-        <v>-1.6716827230632201</v>
+        <f>D154-C154</f>
+        <v>1</v>
       </c>
       <c r="F154" s="2">
-        <f ca="1">E153</f>
-        <v>-0.41272693642897518</v>
+        <f>E153</f>
+        <v>2</v>
       </c>
       <c r="G154" s="2">
-        <f ca="1"/>
-        <v>0.4654162026624068</v>
+        <v>0.8</v>
       </c>
       <c r="H154" s="2">
-        <f ca="1"/>
-        <v>0.88509194906478816</v>
+        <v>-0.60000000000000009</v>
       </c>
       <c r="I154" s="2">
-        <f ca="1"/>
-        <v>7.220716296458074E-2</v>
+        <v>-0.8</v>
       </c>
       <c r="K154" s="2">
-        <f ca="1"/>
-        <v>0</v>
+        <v>-1.1102230246251565E-16</v>
       </c>
       <c r="L154" s="2">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C155" s="24"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="24"/>
+      <c r="F155" s="24"/>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B156" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C156" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G156" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2" t="s">
-        <v>120</v>
+      <c r="H156" s="2"/>
+      <c r="I156" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="K156" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L156" s="22"/>
     </row>
@@ -38749,24 +38722,36 @@
         <v>107</v>
       </c>
       <c r="C157" s="2">
-        <f t="array" aca="1" ref="C157:D158" ca="1">G141:H142</f>
-        <v>-0.49634684237358995</v>
+        <v>0</v>
       </c>
       <c r="D157" s="2">
-        <f ca="1"/>
-        <v>0.86812430680506059</v>
+        <v>1</v>
       </c>
       <c r="E157" s="2">
-        <f t="array" aca="1" ref="E157:E158" ca="1">I141:I142</f>
-        <v>0.26170857228315453</v>
+        <f>D157-C157</f>
+        <v>1</v>
+      </c>
+      <c r="F157" s="2">
+        <f>-E158</f>
+        <v>-1</v>
+      </c>
+      <c r="G157" s="2">
+        <f t="array" ref="G157:H158">{1,0;0,1}-2*(F157:F158*TRANSPOSE(F157:F158))/(F157^2+F158^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H157" s="2">
+        <v>1</v>
+      </c>
+      <c r="I157" s="2">
+        <f t="array" ref="I157:I158">2*F157:F158*SUMPRODUCT(F157:F158,C157:C158)/(F157^2+F158^2)</f>
+        <v>1</v>
       </c>
       <c r="K157" s="17">
-        <f t="array" aca="1" ref="K157:L158" ca="1">MMULT(TRANSPOSE(C157:D158),C157:D158)</f>
-        <v>1.0000000000000002</v>
+        <f t="array" ref="K157:L158">MMULT(G157:H158,G157:H158)</f>
+        <v>1</v>
       </c>
       <c r="L157" s="17">
-        <f ca="1"/>
-        <v>-1.1102230246251565E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.4">
@@ -38774,39 +38759,60 @@
         <v>108</v>
       </c>
       <c r="C158" s="2">
-        <f ca="1"/>
-        <v>0.86812430680506059</v>
+        <v>-1</v>
       </c>
       <c r="D158" s="2">
-        <f ca="1"/>
-        <v>0.49634684237358984</v>
+        <v>0</v>
       </c>
       <c r="E158" s="2">
-        <f ca="1"/>
-        <v>-0.1518334963957054</v>
+        <f>D158-C158</f>
+        <v>1</v>
+      </c>
+      <c r="F158" s="2">
+        <f>E157</f>
+        <v>1</v>
+      </c>
+      <c r="G158" s="2">
+        <v>1</v>
+      </c>
+      <c r="H158" s="2">
+        <v>0</v>
+      </c>
+      <c r="I158" s="2">
+        <v>-1</v>
       </c>
       <c r="K158" s="2">
-        <f ca="1"/>
-        <v>-1.1102230246251565E-16</v>
+        <v>0</v>
       </c>
       <c r="L158" s="2">
-        <f ca="1"/>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B160" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C160" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G160" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2" t="s">
-        <v>120</v>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="K160" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L160" s="22"/>
     </row>
@@ -38815,24 +38821,36 @@
         <v>107</v>
       </c>
       <c r="C161" s="2">
-        <f t="array" aca="1" ref="C161:D162" ca="1">MMULT(G145:H146,C157:D158)</f>
-        <v>-0.77001360893029913</v>
+        <v>0.5</v>
       </c>
       <c r="D161" s="2">
-        <f ca="1"/>
-        <v>0.63802746184011294</v>
+        <v>1</v>
       </c>
       <c r="E161" s="2">
-        <f t="array" aca="1" ref="E161:E162" ca="1">I145:I146+MMULT(C161:D162,E157:E158)</f>
-        <v>-3.2849961554107077E-2</v>
+        <f>D161-C161</f>
+        <v>0.5</v>
+      </c>
+      <c r="F161" s="2">
+        <f>-E162</f>
+        <v>-0.5</v>
+      </c>
+      <c r="G161" s="2">
+        <f t="array" ref="G161:H162">{1,0;0,1}-2*(F161:F162*TRANSPOSE(F161:F162))/(F161^2+F162^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H161" s="2">
+        <v>1</v>
+      </c>
+      <c r="I161" s="2">
+        <f t="array" ref="I161:I162">2*F161:F162*SUMPRODUCT(F161:F162,C161:C162)/(F161^2+F162^2)</f>
+        <v>1.5</v>
       </c>
       <c r="K161" s="17">
-        <f t="array" aca="1" ref="K161:L162" ca="1">MMULT(TRANSPOSE(C161:D162),C161:D162)</f>
-        <v>1.0000000000000004</v>
+        <f t="array" ref="K161:L162">MMULT(G161:H162,G161:H162)</f>
+        <v>1</v>
       </c>
       <c r="L161" s="17">
-        <f ca="1"/>
-        <v>-2.2204460492503131E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.4">
@@ -38840,29 +38858,38 @@
         <v>108</v>
       </c>
       <c r="C162" s="2">
-        <f ca="1"/>
-        <v>-0.63802746184011283</v>
+        <v>-1</v>
       </c>
       <c r="D162" s="2">
-        <f ca="1"/>
-        <v>-0.77001360893029891</v>
+        <v>-0.5</v>
       </c>
       <c r="E162" s="2">
-        <f ca="1"/>
-        <v>1.4113792046898264</v>
+        <f>D162-C162</f>
+        <v>0.5</v>
+      </c>
+      <c r="F162" s="2">
+        <f>E161</f>
+        <v>0.5</v>
+      </c>
+      <c r="G162" s="2">
+        <v>1</v>
+      </c>
+      <c r="H162" s="2">
+        <v>0</v>
+      </c>
+      <c r="I162" s="2">
+        <v>-1.5</v>
       </c>
       <c r="K162" s="2">
-        <f ca="1"/>
-        <v>-2.2204460492503131E-16</v>
+        <v>0</v>
       </c>
       <c r="L162" s="2">
-        <f ca="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B164" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>113</v>
@@ -38881,24 +38908,22 @@
         <v>107</v>
       </c>
       <c r="C165" s="2">
-        <f t="array" aca="1" ref="C165:D166" ca="1">MMULT(G149:H150,C161:D162)</f>
-        <v>-0.99244854123758064</v>
+        <f t="array" ref="C165:D166">G149:H150</f>
+        <v>0</v>
       </c>
       <c r="D165" s="2">
-        <f ca="1"/>
-        <v>-0.12266170142060789</v>
+        <v>1</v>
       </c>
       <c r="E165" s="2">
-        <f t="array" aca="1" ref="E165:E166" ca="1">I149:I150+MMULT(C165:D166,E161:E162)</f>
-        <v>-0.37143636520143775</v>
+        <f t="array" ref="E165:E166">I149:I150</f>
+        <v>0</v>
       </c>
       <c r="K165" s="17">
-        <f t="array" aca="1" ref="K165:L166" ca="1">MMULT(TRANSPOSE(C165:D166),C165:D166)</f>
-        <v>1.0000000000000002</v>
+        <f t="array" ref="K165:L166">MMULT(TRANSPOSE(C165:D166),C165:D166)</f>
+        <v>1</v>
       </c>
       <c r="L165" s="17">
-        <f ca="1"/>
-        <v>-3.6082248300317588E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.4">
@@ -38906,39 +38931,32 @@
         <v>108</v>
       </c>
       <c r="C166" s="2">
-        <f ca="1"/>
-        <v>-0.12266170142060828</v>
+        <v>1</v>
       </c>
       <c r="D166" s="2">
-        <f ca="1"/>
-        <v>0.99244854123758053</v>
+        <v>0</v>
       </c>
       <c r="E166" s="2">
-        <f ca="1"/>
-        <v>1.9397666517017962</v>
+        <v>0</v>
       </c>
       <c r="K166" s="2">
-        <f ca="1"/>
-        <v>-3.6082248300317588E-16</v>
+        <v>0</v>
       </c>
       <c r="L166" s="2">
-        <f ca="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B168" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C168" s="5" t="s">
+      <c r="B168" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D168" s="22"/>
-      <c r="E168" s="22" t="s">
+      <c r="D168" s="2"/>
+      <c r="E168" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G168" s="24"/>
-      <c r="H168" s="24"/>
       <c r="K168" s="5" t="s">
         <v>123</v>
       </c>
@@ -38948,27 +38966,23 @@
       <c r="B169" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C169" s="17">
-        <f t="array" aca="1" ref="C169:D170" ca="1">MMULT(G153:H154,C165:D166)</f>
-        <v>0.82131947042318665</v>
-      </c>
-      <c r="D169" s="17">
-        <f ca="1"/>
-        <v>0.57046851578660873</v>
+      <c r="C169" s="2">
+        <f t="array" ref="C169:D170">MMULT(G153:H154,C165:D166)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D169" s="2">
+        <v>0.6</v>
       </c>
       <c r="E169" s="2">
-        <f t="array" aca="1" ref="E169:E170" ca="1">I153:I154+MMULT(C169:D170,E165:E166)</f>
-        <v>0.50904462039183018</v>
-      </c>
-      <c r="G169" s="24"/>
-      <c r="H169" s="24"/>
+        <f t="array" ref="E169:E170">I153:I154+MMULT(C153:D154,E165:E166)</f>
+        <v>0.4</v>
+      </c>
       <c r="K169" s="17">
-        <f t="array" aca="1" ref="K169:L170" ca="1">MMULT(TRANSPOSE(C169:D170),C169:D170)</f>
-        <v>1.0000000000000004</v>
+        <f t="array" ref="K169:L170">MMULT(TRANSPOSE(C169:D170),C169:D170)</f>
+        <v>1.0000000000000002</v>
       </c>
       <c r="L169" s="17">
-        <f ca="1"/>
-        <v>-2.7755575615628914E-16</v>
+        <v>-1.1102230246251565E-16</v>
       </c>
     </row>
     <row r="170" spans="2:12" x14ac:dyDescent="0.4">
@@ -38976,312 +38990,408 @@
         <v>108</v>
       </c>
       <c r="C170" s="2">
-        <f ca="1"/>
-        <v>-0.57046851578660907</v>
+        <v>-0.60000000000000009</v>
       </c>
       <c r="D170" s="2">
-        <f ca="1"/>
-        <v>0.82131947042318665</v>
+        <v>0.8</v>
       </c>
       <c r="E170" s="2">
-        <f ca="1"/>
-        <v>1.8772680340504948</v>
-      </c>
-      <c r="G170" s="24"/>
-      <c r="H170" s="24"/>
+        <v>-0.8</v>
+      </c>
       <c r="K170" s="2">
-        <f ca="1"/>
-        <v>-2.7755575615628914E-16</v>
+        <v>-1.1102230246251565E-16</v>
       </c>
       <c r="L170" s="2">
-        <f ca="1"/>
         <v>1</v>
       </c>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B172" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D172" s="2"/>
+      <c r="E172" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K172" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L172" s="22"/>
     </row>
     <row r="173" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B173" t="s">
-        <v>127</v>
+      <c r="B173" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C173" s="2">
+        <f t="array" ref="C173:D174">MMULT(G157:H158,C169:D170)</f>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="D173" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E173" s="2">
+        <f t="array" ref="E173:E174">I157:I158+MMULT(C157:D158,E169:E170)</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="K173" s="17">
+        <f t="array" ref="K173:L174">MMULT(TRANSPOSE(C173:D174),C173:D174)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="L173" s="17">
+        <v>-1.1102230246251565E-16</v>
       </c>
     </row>
     <row r="174" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="C174" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F174" s="24"/>
-      <c r="G174" s="24"/>
-      <c r="H174" s="24"/>
-    </row>
-    <row r="175" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B175" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C175" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.138764837597531</v>
-      </c>
-      <c r="D175" s="2">
-        <f t="shared" ref="D175:E176" ca="1" si="0">2*RAND()-1</f>
-        <v>0.36387285617567211</v>
-      </c>
-      <c r="E175" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-0.79728643537602606</v>
+      <c r="B174" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C174" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D174" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E174" s="2">
+        <v>-1.4</v>
+      </c>
+      <c r="K174" s="2">
+        <v>-1.1102230246251565E-16</v>
+      </c>
+      <c r="L174" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B176" s="2" t="s">
+      <c r="B176" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D176" s="22"/>
+      <c r="E176" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="G176" s="24"/>
+      <c r="H176" s="24"/>
+      <c r="K176" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L176" s="22"/>
+    </row>
+    <row r="177" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B177" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C177" s="53">
+        <f t="array" ref="C177:D178">MMULT(G161:H162,C173:D174)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D177" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="E177" s="2">
+        <f t="array" ref="E177:E178">I161:I162+MMULT(C161:D162,E173:E174)</f>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="G177" s="24"/>
+      <c r="H177" s="24"/>
+      <c r="K177" s="17">
+        <f t="array" ref="K177:L178">MMULT(TRANSPOSE(C177:D178),C177:D178)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="L177" s="17">
+        <v>-1.1102230246251565E-16</v>
+      </c>
+    </row>
+    <row r="178" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B178" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C178" s="2">
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="D178" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E178" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G178" s="24"/>
+      <c r="H178" s="24"/>
+      <c r="K178" s="2">
+        <v>-1.1102230246251565E-16</v>
+      </c>
+      <c r="L178" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B181" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="182" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C182" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F182" s="24"/>
+      <c r="G182" s="24"/>
+      <c r="H182" s="24"/>
+    </row>
+    <row r="183" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B183" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C183" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D183" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E183" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B184" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C176" s="2">
-        <f ca="1">2*RAND()-1</f>
-        <v>0.35725188541231967</v>
-      </c>
-      <c r="D176" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1319341123135287</v>
-      </c>
-      <c r="E176" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5823618789290359</v>
+      <c r="C184" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D184" s="2">
+        <v>1</v>
+      </c>
+      <c r="E184" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C178" s="2" t="s">
+    <row r="186" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C186" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D178" s="2" t="s">
+      <c r="D186" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E178" s="2" t="s">
+      <c r="E186" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B179" s="2" t="s">
+    <row r="187" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B187" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C179" s="2">
-        <f t="array" aca="1" ref="C179:C180" ca="1">MMULT($C$169:$D$170,C175:C176)+$E$169:$E$170</f>
-        <v>0.82681583615392751</v>
-      </c>
-      <c r="D179" s="2">
-        <f t="array" aca="1" ref="D179:D180" ca="1">MMULT($C$169:$D$170,D175:D176)+$E$169:$E$170</f>
-        <v>0.88316473916052796</v>
-      </c>
-      <c r="E179" s="2">
-        <f t="array" aca="1" ref="E179:E180" ca="1">MMULT($C$169:$D$170,E175:E176)+$E$169:$E$170</f>
-        <v>0.18643686423655009</v>
+      <c r="C187" s="2">
+        <f t="array" ref="C187:C188">MMULT($C$177:$D$178,C183:C184)+$E$177:$E$178</f>
+        <v>-1.1999999999999997</v>
+      </c>
+      <c r="D187" s="2">
+        <f t="array" ref="D187:D188">MMULT($C$177:$D$178,D183:D184)+$E$177:$E$178</f>
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="E187" s="2">
+        <f t="array" ref="E187:E188">MMULT($C$177:$D$178,E183:E184)+$E$177:$E$178</f>
+        <v>1.6</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B180" s="2" t="s">
+    <row r="188" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B188" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C180" s="2">
-        <f ca="1"/>
-        <v>2.0915249924373929</v>
-      </c>
-      <c r="D180" s="2">
-        <f ca="1"/>
-        <v>1.7780500811090254</v>
-      </c>
-      <c r="E180" s="2">
-        <f ca="1"/>
-        <v>2.8103999934929003</v>
+      <c r="C188" s="2">
+        <v>-1.2</v>
+      </c>
+      <c r="D188" s="2">
+        <v>0.40000000000000013</v>
+      </c>
+      <c r="E188" s="2">
+        <v>-0.8</v>
       </c>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C183" s="2" t="s">
+    <row r="191" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C191" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D183" s="2" t="s">
+      <c r="D191" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E183" s="24"/>
-      <c r="F183" s="29"/>
+      <c r="E191" s="24"/>
+      <c r="F191" s="29"/>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B184" s="2" t="s">
+    <row r="192" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B192" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C184" s="2">
-        <f t="array" aca="1" ref="C184:C185" ca="1">D175:D176-C175:C176</f>
-        <v>0.22510801857814111</v>
-      </c>
-      <c r="D184" s="2">
-        <f t="array" aca="1" ref="D184:D185" ca="1">E175:E176-C175:C176</f>
-        <v>-0.93605127297355706</v>
-      </c>
-      <c r="E184" s="24"/>
-      <c r="F184" s="24"/>
+      <c r="C192" s="2">
+        <f t="array" ref="C192:C193">D183:D184-C183:C184</f>
+        <v>0</v>
+      </c>
+      <c r="D192" s="2">
+        <f t="array" ref="D192:D193">E183:E184-C183:C184</f>
+        <v>2</v>
+      </c>
+      <c r="E192" s="52"/>
+      <c r="F192" s="24"/>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B185" s="2" t="s">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B193" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C185" s="2">
-        <f ca="1"/>
-        <v>-0.22531777309879097</v>
-      </c>
-      <c r="D185" s="2">
-        <f ca="1"/>
-        <v>0.22510999351671623</v>
-      </c>
-      <c r="E185" s="24"/>
-      <c r="F185" s="24"/>
+      <c r="C193" s="2">
+        <v>2</v>
+      </c>
+      <c r="D193" s="2">
+        <v>2</v>
+      </c>
+      <c r="E193" s="24"/>
+      <c r="F193" s="24"/>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C187" s="2" t="s">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C195" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D187" s="2" t="s">
+      <c r="D195" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E187" s="2" t="s">
+      <c r="E195" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F187" s="2" t="s">
+      <c r="F195" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B188" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C188" s="2">
-        <f t="array" aca="1" ref="C188:C189" ca="1">D179:D180-C179:C180</f>
-        <v>5.6348903006600448E-2</v>
-      </c>
-      <c r="D188" s="2">
-        <f t="array" aca="1" ref="D188:D189" ca="1">E179:E180-C179:C180</f>
-        <v>-0.64037897191737736</v>
-      </c>
-      <c r="E188" s="2">
-        <f ca="1">-C189</f>
-        <v>0.31347491132836747</v>
-      </c>
-      <c r="F188" s="2">
-        <f ca="1">-D189</f>
-        <v>-0.71887500105550739</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B189" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C189" s="2">
-        <f ca="1"/>
-        <v>-0.31347491132836747</v>
-      </c>
-      <c r="D189" s="2">
-        <f ca="1"/>
-        <v>0.71887500105550739</v>
-      </c>
-      <c r="E189" s="2">
-        <f ca="1">C188</f>
-        <v>5.6348903006600448E-2</v>
-      </c>
-      <c r="F189" s="2">
-        <f ca="1">D188</f>
-        <v>-0.64037897191737736</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B191" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C191" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D191" s="22"/>
-      <c r="E191" s="22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B192" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C192" s="17">
-        <f t="array" aca="1" ref="C192:D193" ca="1">1/SUMPRODUCT(E188:E189,D188:D189)*(E188:E189*TRANSPOSE(D184:D185)-F188:F189*TRANSPOSE(C184:C185))</f>
-        <v>0.82131947042318654</v>
-      </c>
-      <c r="D192" s="17">
-        <f ca="1"/>
-        <v>0.57046851578660807</v>
-      </c>
-      <c r="E192" s="2">
-        <f t="array" aca="1" ref="E192:E193" ca="1">C179:C180-MMULT(C192:D193,C175:C176)</f>
-        <v>0.50904462039183052</v>
-      </c>
-    </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B193" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C193" s="2">
-        <f ca="1"/>
-        <v>-0.57046851578660873</v>
-      </c>
-      <c r="D193" s="2">
-        <f ca="1"/>
-        <v>0.82131947042318565</v>
-      </c>
-      <c r="E193" s="2">
-        <f ca="1"/>
-        <v>1.8772680340504952</v>
-      </c>
-    </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B195" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C195" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D195" s="22"/>
-      <c r="E195" s="22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B196" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C196" s="30">
-        <f t="array" aca="1" ref="C196:D197" ca="1">C169:D170-C192:D193</f>
-        <v>1.1102230246251565E-16</v>
-      </c>
-      <c r="D196" s="30">
-        <f ca="1"/>
-        <v>6.6613381477509392E-16</v>
-      </c>
-      <c r="E196" s="31">
-        <f t="array" aca="1" ref="E196:E197" ca="1">E169:E170-E192:E193</f>
-        <v>-3.3306690738754696E-16</v>
+      <c r="C196" s="2">
+        <f t="array" ref="C196:C197">D187:D188-C187:C188</f>
+        <v>1.1999999999999997</v>
+      </c>
+      <c r="D196" s="2">
+        <f t="array" ref="D196:D197">E187:E188-C187:C188</f>
+        <v>2.8</v>
+      </c>
+      <c r="E196" s="2">
+        <f>-C197</f>
+        <v>-1.6</v>
+      </c>
+      <c r="F196" s="2">
+        <f>-D197</f>
+        <v>-0.39999999999999991</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B197" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C197" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D197" s="2">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E197" s="2">
+        <f>C196</f>
+        <v>1.1999999999999997</v>
+      </c>
+      <c r="F197" s="2">
+        <f>D196</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="199" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B199" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D199" s="22"/>
+      <c r="E199" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="200" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B200" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C200" s="17">
+        <f t="array" ref="C200:D201">1/SUMPRODUCT(E196:E197,D196:D197)*(E196:E197*TRANSPOSE(D192:D193)-F196:F197*TRANSPOSE(C192:C193))</f>
+        <v>0.8</v>
+      </c>
+      <c r="D200" s="17">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E200" s="2">
+        <f t="array" ref="E200:E201">C187:C188-MMULT(C200:D201,C183:C184)</f>
+        <v>0.2000000000000004</v>
+      </c>
+    </row>
+    <row r="201" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B201" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C201" s="2">
+        <v>-0.59999999999999987</v>
+      </c>
+      <c r="D201" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E201" s="2">
+        <v>-0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="203" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B203" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C203" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C197" s="31">
-        <f ca="1"/>
-        <v>-3.3306690738754696E-16</v>
-      </c>
-      <c r="D197" s="31">
-        <f ca="1"/>
-        <v>9.9920072216264089E-16</v>
-      </c>
-      <c r="E197" s="31">
-        <f ca="1"/>
-        <v>-4.4408920985006262E-16</v>
+      <c r="D203" s="22"/>
+      <c r="E203" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B204" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C204" s="30">
+        <f t="array" ref="C204:D205">C177:D178-C200:D201</f>
+        <v>0</v>
+      </c>
+      <c r="D204" s="30">
+        <v>0</v>
+      </c>
+      <c r="E204" s="31">
+        <f t="array" ref="E204:E205">E177:E178-E200:E201</f>
+        <v>-2.2204460492503131E-16</v>
+      </c>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B205" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C205" s="31">
+        <v>0</v>
+      </c>
+      <c r="D205" s="31">
+        <v>0</v>
+      </c>
+      <c r="E205" s="31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -39373,18 +39483,18 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B12" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="37" t="s">
         <v>155</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>156</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
@@ -39567,21 +39677,21 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B24" s="37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="37" t="s">
         <v>75</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
@@ -39710,7 +39820,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H32" s="24"/>
       <c r="I32" s="29"/>
@@ -39723,63 +39833,63 @@
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
       <c r="I33" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J33" s="36"/>
       <c r="K33" s="32"/>
       <c r="P33" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q33" s="48"/>
       <c r="R33" s="22"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B34" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34" s="27" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="M34" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="M34" s="3" t="s">
+      <c r="N34" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="N34" s="3" t="s">
+      <c r="O34" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="O34" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="P34" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q34" s="22"/>
       <c r="R34" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.4">
@@ -41147,12 +41257,12 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B70" s="42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C70" s="2">
         <v>2</v>
@@ -41160,7 +41270,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C72" s="42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D72" s="42">
         <f>C70</f>
@@ -41186,7 +41296,7 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C73" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
@@ -41211,10 +41321,10 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="42" t="s">
         <v>167</v>
-      </c>
-      <c r="C74" s="42" t="s">
-        <v>168</v>
       </c>
       <c r="D74" s="2">
         <f>INDEX($D$13:$D$21,MATCH(D72,$B$13:$B$21,0)+D73-1)</f>
@@ -41240,7 +41350,7 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B75" s="42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C75" s="42">
         <v>1</v>
@@ -41353,12 +41463,12 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B81" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C81" s="42">
         <v>1</v>

</xml_diff>